<commit_message>
added excel util class
</commit_message>
<xml_diff>
--- a/vytrack_testusers.xlsx
+++ b/vytrack_testusers.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marufjon/Downloads/"/>
     </mc:Choice>
@@ -22,7 +22,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3863" uniqueCount="1478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3865" uniqueCount="1479">
   <si>
     <t>username</t>
   </si>
@@ -4470,12 +4470,16 @@
   </si>
   <si>
     <t>n/a</t>
+  </si>
+  <si>
+    <t>PASSED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -4829,8 +4833,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -9073,8 +9077,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -9364,8 +9368,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -13611,8 +13615,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -13646,7 +13650,7 @@
         <v>305</v>
       </c>
       <c r="E2" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -13902,8 +13906,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -18149,8 +18153,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>